<commit_message>
spev v4 number 2
</commit_message>
<xml_diff>
--- a/resource/SPEC Salmon ของน้องอ้วน V4.1.xlsx
+++ b/resource/SPEC Salmon ของน้องอ้วน V4.1.xlsx
@@ -1282,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="J115" sqref="J115"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1296,7 +1296,7 @@
     <col min="6" max="6" width="51.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
         <v>49</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1341,8 +1341,11 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1355,8 +1358,11 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1366,8 +1372,11 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1377,8 +1386,11 @@
       <c r="E6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1388,8 +1400,11 @@
       <c r="E7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1399,8 +1414,11 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" s="5" customFormat="1">
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="5" customFormat="1">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -1410,8 +1428,11 @@
       <c r="E9" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="5" customFormat="1">
+      <c r="G9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="5" customFormat="1">
       <c r="A10" s="5" t="s">
         <v>2</v>
       </c>
@@ -1424,8 +1445,11 @@
       <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="5" customFormat="1">
+      <c r="G10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="5" customFormat="1">
       <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
@@ -1438,8 +1462,11 @@
       <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="5" customFormat="1">
+      <c r="G11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="5" customFormat="1">
       <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
@@ -1449,8 +1476,11 @@
       <c r="E12" s="5" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" s="5" customFormat="1">
+      <c r="G12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="5" customFormat="1">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -1463,8 +1493,11 @@
       <c r="D13" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" s="5" customFormat="1">
+      <c r="G13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1">
       <c r="A14" s="5" t="s">
         <v>2</v>
       </c>
@@ -1474,8 +1507,11 @@
       <c r="E14" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" s="5" customFormat="1">
+      <c r="G14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="5" customFormat="1">
       <c r="A15" s="5" t="s">
         <v>2</v>
       </c>
@@ -1485,8 +1521,11 @@
       <c r="E15" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" s="5" customFormat="1">
+      <c r="G15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="5" customFormat="1">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
@@ -1496,8 +1535,11 @@
       <c r="E16" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" s="5" customFormat="1">
+      <c r="G16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="5" customFormat="1">
       <c r="A17" s="5" t="s">
         <v>2</v>
       </c>
@@ -1507,8 +1549,11 @@
       <c r="E17" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" s="5" customFormat="1">
+      <c r="G17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="5" customFormat="1">
       <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
@@ -1521,8 +1566,11 @@
       <c r="D18" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" s="5" customFormat="1">
+      <c r="G18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="5" customFormat="1">
       <c r="A19" s="5" t="s">
         <v>2</v>
       </c>
@@ -1532,8 +1580,11 @@
       <c r="E19" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" s="5" customFormat="1">
+      <c r="G19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="5" customFormat="1">
       <c r="A20" s="5" t="s">
         <v>2</v>
       </c>
@@ -1543,8 +1594,11 @@
       <c r="E20" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" s="5" customFormat="1">
+      <c r="G20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="5" customFormat="1">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -1554,8 +1608,11 @@
       <c r="E21" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" s="5" customFormat="1">
+      <c r="G21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="5" customFormat="1">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -1565,8 +1622,11 @@
       <c r="E22" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" s="5" customFormat="1">
+      <c r="G22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="5" customFormat="1">
       <c r="A23" s="5" t="s">
         <v>2</v>
       </c>
@@ -1576,8 +1636,11 @@
       <c r="E23" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" s="5" customFormat="1">
+      <c r="G23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="5" customFormat="1">
       <c r="A24" s="5" t="s">
         <v>2</v>
       </c>
@@ -1587,8 +1650,11 @@
       <c r="E24" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" s="5" customFormat="1">
+      <c r="G24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="5" customFormat="1">
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
@@ -1598,8 +1664,11 @@
       <c r="E25" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" s="5" customFormat="1">
+      <c r="G25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="5" customFormat="1">
       <c r="A26" s="5" t="s">
         <v>2</v>
       </c>
@@ -1612,8 +1681,11 @@
       <c r="D26" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" s="5" customFormat="1">
+      <c r="G26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="5" customFormat="1">
       <c r="A27" s="5" t="s">
         <v>2</v>
       </c>
@@ -1623,8 +1695,11 @@
       <c r="E27" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" s="5" customFormat="1">
+      <c r="G27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="5" customFormat="1">
       <c r="A28" s="5" t="s">
         <v>2</v>
       </c>
@@ -1637,8 +1712,11 @@
       <c r="D28" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" s="5" customFormat="1">
+      <c r="G28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="5" customFormat="1">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
@@ -1648,8 +1726,11 @@
       <c r="E29" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" s="5" customFormat="1">
+      <c r="G29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="5" customFormat="1">
       <c r="A30" s="5" t="s">
         <v>2</v>
       </c>
@@ -1659,8 +1740,11 @@
       <c r="E30" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" s="5" customFormat="1">
+      <c r="G30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="5" customFormat="1">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -1670,8 +1754,11 @@
       <c r="E31" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" s="5" customFormat="1">
+      <c r="G31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="5" customFormat="1">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -1681,8 +1768,11 @@
       <c r="E32" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" s="5" customFormat="1">
+      <c r="G32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="5" customFormat="1">
       <c r="A33" s="5" t="s">
         <v>2</v>
       </c>
@@ -1692,8 +1782,11 @@
       <c r="E33" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" s="5" customFormat="1">
+      <c r="G33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="5" customFormat="1">
       <c r="A34" s="5" t="s">
         <v>60</v>
       </c>
@@ -1707,7 +1800,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="5" customFormat="1">
+    <row r="35" spans="1:7" s="5" customFormat="1">
       <c r="A35" s="5" t="s">
         <v>60</v>
       </c>
@@ -1721,7 +1814,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="5" customFormat="1">
+    <row r="36" spans="1:7" s="5" customFormat="1">
       <c r="A36" s="5" t="s">
         <v>60</v>
       </c>
@@ -1735,7 +1828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="5" customFormat="1">
+    <row r="37" spans="1:7" s="5" customFormat="1">
       <c r="A37" s="5" t="s">
         <v>60</v>
       </c>
@@ -1749,7 +1842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="5" customFormat="1">
+    <row r="38" spans="1:7" s="5" customFormat="1">
       <c r="A38" s="5" t="s">
         <v>60</v>
       </c>
@@ -1760,7 +1853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="5" customFormat="1">
+    <row r="39" spans="1:7" s="5" customFormat="1">
       <c r="A39" s="5" t="s">
         <v>60</v>
       </c>
@@ -1771,7 +1864,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="5" customFormat="1">
+    <row r="40" spans="1:7" s="5" customFormat="1">
       <c r="A40" s="5" t="s">
         <v>60</v>
       </c>
@@ -1782,7 +1875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="5" customFormat="1">
+    <row r="41" spans="1:7" s="5" customFormat="1">
       <c r="A41" s="5" t="s">
         <v>60</v>
       </c>
@@ -1793,7 +1886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="5" customFormat="1">
+    <row r="42" spans="1:7" s="5" customFormat="1">
       <c r="A42" s="5" t="s">
         <v>60</v>
       </c>
@@ -1804,7 +1897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="5" customFormat="1">
+    <row r="43" spans="1:7" s="5" customFormat="1">
       <c r="A43" s="5" t="s">
         <v>60</v>
       </c>
@@ -1815,7 +1908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="5" customFormat="1">
+    <row r="44" spans="1:7" s="5" customFormat="1">
       <c r="A44" s="5" t="s">
         <v>60</v>
       </c>
@@ -1826,7 +1919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="5" customFormat="1">
+    <row r="45" spans="1:7" s="5" customFormat="1">
       <c r="A45" s="5" t="s">
         <v>60</v>
       </c>
@@ -1837,7 +1930,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="5" customFormat="1">
+    <row r="46" spans="1:7" s="5" customFormat="1">
       <c r="A46" s="5" t="s">
         <v>60</v>
       </c>
@@ -1848,7 +1941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="5" customFormat="1">
+    <row r="47" spans="1:7" s="5" customFormat="1">
       <c r="A47" s="5" t="s">
         <v>60</v>
       </c>
@@ -1859,7 +1952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="5" customFormat="1">
+    <row r="48" spans="1:7" s="5" customFormat="1">
       <c r="A48" s="5" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
check PLNNR, PLNAL, SLWBEZ
</commit_message>
<xml_diff>
--- a/resource/SPEC Salmon ของน้องอ้วน V4.1.xlsx
+++ b/resource/SPEC Salmon ของน้องอ้วน V4.1.xlsx
@@ -1282,18 +1282,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>